<commit_message>
Added raw metrics data
</commit_message>
<xml_diff>
--- a/metrics_causal.xlsx
+++ b/metrics_causal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amogh/Academic/Cambridge/L65/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{531B6BF5-B582-8047-97F4-C476ADEF589D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D61AEF6-6526-9947-90A0-8A0784D88DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{CAC718FA-1DA9-5F4A-B975-0FDA83AFA7A5}"/>
   </bookViews>
@@ -142,6 +142,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{525C791E-E200-9F47-9986-671C8211C198}" name="Table1" displayName="Table1" ref="A2:D11" totalsRowShown="0">
+  <autoFilter ref="A2:D11" xr:uid="{525C791E-E200-9F47-9986-671C8211C198}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{642A03E1-23CB-D54B-919E-6C1C817F2EB6}" name="Algorithm"/>
+    <tableColumn id="2" xr3:uid="{CF16973B-7F0A-D145-A502-D6484265D2A9}" name="Data Split"/>
+    <tableColumn id="3" xr3:uid="{FD7B666C-E9AD-E643-BE08-C55DB588BB3B}" name="Metric"/>
+    <tableColumn id="4" xr3:uid="{FC83F424-215E-AA4A-AC2B-8CD32292B84B}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA85290A-6E39-8A4B-B269-CE5327683448}" name="Table2" displayName="Table2" ref="A14:D23" totalsRowShown="0">
+  <autoFilter ref="A14:D23" xr:uid="{CA85290A-6E39-8A4B-B269-CE5327683448}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6F8C50E6-A343-664C-B4A7-30CACC39318D}" name="Algorithm"/>
+    <tableColumn id="2" xr3:uid="{EB177EF6-3254-4B43-9F6D-96ECC1298EF5}" name="Data Split"/>
+    <tableColumn id="3" xr3:uid="{89CBBDB9-51CA-B744-9B1F-7CCBD8CD38DF}" name="Metric"/>
+    <tableColumn id="4" xr3:uid="{BFF85BB6-E14F-4E4A-B422-4E4400405E32}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67682E5C-9DDD-4C48-B1F5-3FFEE50E2AC7}" name="Table3" displayName="Table3" ref="A26:D35" totalsRowShown="0">
+  <autoFilter ref="A26:D35" xr:uid="{67682E5C-9DDD-4C48-B1F5-3FFEE50E2AC7}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A8D7FD46-B258-6640-915F-32E77077627A}" name="Algorithm"/>
+    <tableColumn id="2" xr3:uid="{5C18443D-FD1B-7444-BEB4-54DED2F733F1}" name="Data Split"/>
+    <tableColumn id="3" xr3:uid="{73B76E2A-0A21-184D-90F9-0AA2631E0345}" name="Metric"/>
+    <tableColumn id="4" xr3:uid="{F22DF696-CD26-BC43-A851-CCA214400BDF}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6BCE01CB-3623-F943-A631-0020DDEDFDC2}" name="Table4" displayName="Table4" ref="A38:D47" totalsRowShown="0">
+  <autoFilter ref="A38:D47" xr:uid="{6BCE01CB-3623-F943-A631-0020DDEDFDC2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{707CCD0D-1A62-0443-A9FA-99DC0FA0F28E}" name="Algorithm"/>
+    <tableColumn id="2" xr3:uid="{5C59C8DD-82BC-C84A-852B-297D85B81CB3}" name="Data Split"/>
+    <tableColumn id="3" xr3:uid="{C981E56D-AF12-0541-ADBD-62362823CB43}" name="Metric"/>
+    <tableColumn id="4" xr3:uid="{E37D5B75-E777-B342-9511-8F15A212B546}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,10 +516,16 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:D47"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1051,5 +1109,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>